<commit_message>
AgileJava: Lesson 11: Samples
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\my_document\git\AgileJavaPlaying\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7759CF4F-39A6-497D-909A-3D898FD8DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645B2D31-C44A-4AC4-AFB9-4E4767EAA40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7095E5D2-6A59-4598-8180-DCE44E082B2B}"/>
   </bookViews>
@@ -498,13 +498,13 @@
                   <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>332</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1337,14 +1337,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>652461</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>61911</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -1671,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400697B7-E24B-493D-B1C3-F9F9331F3951}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1683,7 +1683,7 @@
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>16</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1714,8 +1714,12 @@
       <c r="F2">
         <v>237</v>
       </c>
+      <c r="G2">
+        <f>F3-F2</f>
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1732,8 +1736,12 @@
       <c r="F3">
         <v>259</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">F4-F3</f>
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1748,10 +1756,14 @@
         <v>40</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>295</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1766,10 +1778,14 @@
         <v>32</v>
       </c>
       <c r="F5">
+        <v>332</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1784,10 +1800,13 @@
         <v>38</v>
       </c>
       <c r="F6">
+        <v>332</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1804,8 +1823,12 @@
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -1823,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>15</v>
       </c>

</xml_diff>